<commit_message>
new changes added on test branch
</commit_message>
<xml_diff>
--- a/Reports/test.xlsx
+++ b/Reports/test.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="moneycontrol" r:id="rId3" sheetId="1"/>
+    <sheet name="trendlyn" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="985">
   <si>
     <t>Company</t>
   </si>
@@ -1548,6 +1549,1425 @@
   </si>
   <si>
     <t>636,372</t>
+  </si>
+  <si>
+    <t>Bannari A Spg</t>
+  </si>
+  <si>
+    <t>104.55</t>
+  </si>
+  <si>
+    <t>11.45</t>
+  </si>
+  <si>
+    <t>12.30</t>
+  </si>
+  <si>
+    <t>Reliance ETF Ju</t>
+  </si>
+  <si>
+    <t>391.68</t>
+  </si>
+  <si>
+    <t>0.04</t>
+  </si>
+  <si>
+    <t>Bank of Baroda</t>
+  </si>
+  <si>
+    <t>83.85</t>
+  </si>
+  <si>
+    <t>0.36</t>
+  </si>
+  <si>
+    <t>Chaman Lal Seti</t>
+  </si>
+  <si>
+    <t>130.00</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>Den Networks</t>
+  </si>
+  <si>
+    <t>50.90</t>
+  </si>
+  <si>
+    <t>4.62</t>
+  </si>
+  <si>
+    <t>Capri Global</t>
+  </si>
+  <si>
+    <t>462.70</t>
+  </si>
+  <si>
+    <t>1.70</t>
+  </si>
+  <si>
+    <t>0.37</t>
+  </si>
+  <si>
+    <t>Everest Ind</t>
+  </si>
+  <si>
+    <t>402.65</t>
+  </si>
+  <si>
+    <t>11.10</t>
+  </si>
+  <si>
+    <t>2.83</t>
+  </si>
+  <si>
+    <t>Embassy Office</t>
+  </si>
+  <si>
+    <t>327.03</t>
+  </si>
+  <si>
+    <t>0.21</t>
+  </si>
+  <si>
+    <t>HDFC Life</t>
+  </si>
+  <si>
+    <t>668.95</t>
+  </si>
+  <si>
+    <t>4.90</t>
+  </si>
+  <si>
+    <t>0.74</t>
+  </si>
+  <si>
+    <t>Jayaswal Neco</t>
+  </si>
+  <si>
+    <t>18.10</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>1.40</t>
+  </si>
+  <si>
+    <t>Kalyani Invest</t>
+  </si>
+  <si>
+    <t>1,711.30</t>
+  </si>
+  <si>
+    <t>0.43</t>
+  </si>
+  <si>
+    <t>KIOCL</t>
+  </si>
+  <si>
+    <t>246.55</t>
+  </si>
+  <si>
+    <t>4.98</t>
+  </si>
+  <si>
+    <t>Krishana Phosch</t>
+  </si>
+  <si>
+    <t>86.00</t>
+  </si>
+  <si>
+    <t>0.53</t>
+  </si>
+  <si>
+    <t>The Byke Hosp</t>
+  </si>
+  <si>
+    <t>34.20</t>
+  </si>
+  <si>
+    <t>15.74</t>
+  </si>
+  <si>
+    <t>Man Infra</t>
+  </si>
+  <si>
+    <t>47.90</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>0.10</t>
+  </si>
+  <si>
+    <t>Bosch</t>
+  </si>
+  <si>
+    <t>15,104.45</t>
+  </si>
+  <si>
+    <t>0.24</t>
+  </si>
+  <si>
+    <t>Marshall Machin</t>
+  </si>
+  <si>
+    <t>15.75</t>
+  </si>
+  <si>
+    <t>1.94</t>
+  </si>
+  <si>
+    <t>Digispice Tech</t>
+  </si>
+  <si>
+    <t>44.15</t>
+  </si>
+  <si>
+    <t>0.50</t>
+  </si>
+  <si>
+    <t>Pitti Engineeri</t>
+  </si>
+  <si>
+    <t>97.75</t>
+  </si>
+  <si>
+    <t>0.88</t>
+  </si>
+  <si>
+    <t>Petronet LNG</t>
+  </si>
+  <si>
+    <t>240.80</t>
+  </si>
+  <si>
+    <t>0.54</t>
+  </si>
+  <si>
+    <t>PNB</t>
+  </si>
+  <si>
+    <t>42.25</t>
+  </si>
+  <si>
+    <t>Radha Madhav</t>
+  </si>
+  <si>
+    <t>2.55</t>
+  </si>
+  <si>
+    <t>4.08</t>
+  </si>
+  <si>
+    <t>SecUR Credentia</t>
+  </si>
+  <si>
+    <t>23.20</t>
+  </si>
+  <si>
+    <t>1.10</t>
+  </si>
+  <si>
+    <t>Arihant Super</t>
+  </si>
+  <si>
+    <t>74.45</t>
+  </si>
+  <si>
+    <t>1.55</t>
+  </si>
+  <si>
+    <t>2.13</t>
+  </si>
+  <si>
+    <t>Xchanging Sol</t>
+  </si>
+  <si>
+    <t>76.60</t>
+  </si>
+  <si>
+    <t>1.95</t>
+  </si>
+  <si>
+    <t>2.61</t>
+  </si>
+  <si>
+    <t>Sun TV Network</t>
+  </si>
+  <si>
+    <t>546.00</t>
+  </si>
+  <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>Usha Martin Edu</t>
+  </si>
+  <si>
+    <t>4.20</t>
+  </si>
+  <si>
+    <t>0.20</t>
+  </si>
+  <si>
+    <t>5.00</t>
+  </si>
+  <si>
+    <t>V-Guard Ind</t>
+  </si>
+  <si>
+    <t>269.85</t>
+  </si>
+  <si>
+    <t>89.55</t>
+  </si>
+  <si>
+    <t>15.00</t>
+  </si>
+  <si>
+    <t>16.75</t>
+  </si>
+  <si>
+    <t>116,110</t>
+  </si>
+  <si>
+    <t>389.50</t>
+  </si>
+  <si>
+    <t>0.56</t>
+  </si>
+  <si>
+    <t>53,965</t>
+  </si>
+  <si>
+    <t>80.60</t>
+  </si>
+  <si>
+    <t>3.25</t>
+  </si>
+  <si>
+    <t>53,617,303</t>
+  </si>
+  <si>
+    <t>129.05</t>
+  </si>
+  <si>
+    <t>147,199</t>
+  </si>
+  <si>
+    <t>48.10</t>
+  </si>
+  <si>
+    <t>5.82</t>
+  </si>
+  <si>
+    <t>1,064,390</t>
+  </si>
+  <si>
+    <t>460.05</t>
+  </si>
+  <si>
+    <t>2.65</t>
+  </si>
+  <si>
+    <t>0.58</t>
+  </si>
+  <si>
+    <t>114,882</t>
+  </si>
+  <si>
+    <t>388.60</t>
+  </si>
+  <si>
+    <t>14.05</t>
+  </si>
+  <si>
+    <t>66,633</t>
+  </si>
+  <si>
+    <t>322.21</t>
+  </si>
+  <si>
+    <t>4.82</t>
+  </si>
+  <si>
+    <t>262,000</t>
+  </si>
+  <si>
+    <t>658.50</t>
+  </si>
+  <si>
+    <t>10.45</t>
+  </si>
+  <si>
+    <t>1.59</t>
+  </si>
+  <si>
+    <t>1,809,231</t>
+  </si>
+  <si>
+    <t>17.65</t>
+  </si>
+  <si>
+    <t>447,619</t>
+  </si>
+  <si>
+    <t>1,701.20</t>
+  </si>
+  <si>
+    <t>10.10</t>
+  </si>
+  <si>
+    <t>0.59</t>
+  </si>
+  <si>
+    <t>724</t>
+  </si>
+  <si>
+    <t>223.70</t>
+  </si>
+  <si>
+    <t>22.85</t>
+  </si>
+  <si>
+    <t>10.21</t>
+  </si>
+  <si>
+    <t>152,858</t>
+  </si>
+  <si>
+    <t>83.35</t>
+  </si>
+  <si>
+    <t>3.18</t>
+  </si>
+  <si>
+    <t>3,940</t>
+  </si>
+  <si>
+    <t>24.65</t>
+  </si>
+  <si>
+    <t>9.55</t>
+  </si>
+  <si>
+    <t>38.74</t>
+  </si>
+  <si>
+    <t>58,676</t>
+  </si>
+  <si>
+    <t>46.70</t>
+  </si>
+  <si>
+    <t>2.57</t>
+  </si>
+  <si>
+    <t>546,060</t>
+  </si>
+  <si>
+    <t>14,882.35</t>
+  </si>
+  <si>
+    <t>222.10</t>
+  </si>
+  <si>
+    <t>1.49</t>
+  </si>
+  <si>
+    <t>47,060</t>
+  </si>
+  <si>
+    <t>14.75</t>
+  </si>
+  <si>
+    <t>6.78</t>
+  </si>
+  <si>
+    <t>3,000</t>
+  </si>
+  <si>
+    <t>41.60</t>
+  </si>
+  <si>
+    <t>6.13</t>
+  </si>
+  <si>
+    <t>196,600</t>
+  </si>
+  <si>
+    <t>90.15</t>
+  </si>
+  <si>
+    <t>8.43</t>
+  </si>
+  <si>
+    <t>193,759</t>
+  </si>
+  <si>
+    <t>234.50</t>
+  </si>
+  <si>
+    <t>6.30</t>
+  </si>
+  <si>
+    <t>2.69</t>
+  </si>
+  <si>
+    <t>1,716,260</t>
+  </si>
+  <si>
+    <t>39.25</t>
+  </si>
+  <si>
+    <t>3.00</t>
+  </si>
+  <si>
+    <t>7.64</t>
+  </si>
+  <si>
+    <t>91,471,489</t>
+  </si>
+  <si>
+    <t>2.35</t>
+  </si>
+  <si>
+    <t>8.51</t>
+  </si>
+  <si>
+    <t>185,817</t>
+  </si>
+  <si>
+    <t>2.15</t>
+  </si>
+  <si>
+    <t>1,800</t>
+  </si>
+  <si>
+    <t>69.65</t>
+  </si>
+  <si>
+    <t>6.89</t>
+  </si>
+  <si>
+    <t>53,977</t>
+  </si>
+  <si>
+    <t>73.50</t>
+  </si>
+  <si>
+    <t>3.10</t>
+  </si>
+  <si>
+    <t>4.22</t>
+  </si>
+  <si>
+    <t>92,823</t>
+  </si>
+  <si>
+    <t>539.20</t>
+  </si>
+  <si>
+    <t>6.80</t>
+  </si>
+  <si>
+    <t>1.26</t>
+  </si>
+  <si>
+    <t>1,212,391</t>
+  </si>
+  <si>
+    <t>9.09</t>
+  </si>
+  <si>
+    <t>10,938</t>
+  </si>
+  <si>
+    <t>248.90</t>
+  </si>
+  <si>
+    <t>20.95</t>
+  </si>
+  <si>
+    <t>8.42</t>
+  </si>
+  <si>
+    <t>1,084,361</t>
+  </si>
+  <si>
+    <t>72.30</t>
+  </si>
+  <si>
+    <t>0.80</t>
+  </si>
+  <si>
+    <t>1.11</t>
+  </si>
+  <si>
+    <t>99,230</t>
+  </si>
+  <si>
+    <t>Bajaj Finance</t>
+  </si>
+  <si>
+    <t>6,544.10</t>
+  </si>
+  <si>
+    <t>134.00</t>
+  </si>
+  <si>
+    <t>2.09</t>
+  </si>
+  <si>
+    <t>Britannia</t>
+  </si>
+  <si>
+    <t>3,720.75</t>
+  </si>
+  <si>
+    <t>24.25</t>
+  </si>
+  <si>
+    <t>Emami</t>
+  </si>
+  <si>
+    <t>597.45</t>
+  </si>
+  <si>
+    <t>7.30</t>
+  </si>
+  <si>
+    <t>1.24</t>
+  </si>
+  <si>
+    <t>Fortis Health</t>
+  </si>
+  <si>
+    <t>267.75</t>
+  </si>
+  <si>
+    <t>3.15</t>
+  </si>
+  <si>
+    <t>1.19</t>
+  </si>
+  <si>
+    <t>FIEM Ind</t>
+  </si>
+  <si>
+    <t>1,015.65</t>
+  </si>
+  <si>
+    <t>73.20</t>
+  </si>
+  <si>
+    <t>7.77</t>
+  </si>
+  <si>
+    <t>HDFC AMC</t>
+  </si>
+  <si>
+    <t>2,995.90</t>
+  </si>
+  <si>
+    <t>18.15</t>
+  </si>
+  <si>
+    <t>0.61</t>
+  </si>
+  <si>
+    <t>ICICI Prudentia</t>
+  </si>
+  <si>
+    <t>680.70</t>
+  </si>
+  <si>
+    <t>4.40</t>
+  </si>
+  <si>
+    <t>0.65</t>
+  </si>
+  <si>
+    <t>Jai Balaji Ind</t>
+  </si>
+  <si>
+    <t>65.90</t>
+  </si>
+  <si>
+    <t>0.76</t>
+  </si>
+  <si>
+    <t>JK Lakshmi Cem</t>
+  </si>
+  <si>
+    <t>709.50</t>
+  </si>
+  <si>
+    <t>7.75</t>
+  </si>
+  <si>
+    <t>144.05</t>
+  </si>
+  <si>
+    <t>0.07</t>
+  </si>
+  <si>
+    <t>Poonawalla Fin</t>
+  </si>
+  <si>
+    <t>194.40</t>
+  </si>
+  <si>
+    <t>0.60</t>
+  </si>
+  <si>
+    <t>Nestle</t>
+  </si>
+  <si>
+    <t>18,911.00</t>
+  </si>
+  <si>
+    <t>178.45</t>
+  </si>
+  <si>
+    <t>Power Mech</t>
+  </si>
+  <si>
+    <t>852.55</t>
+  </si>
+  <si>
+    <t>Quantum Index</t>
+  </si>
+  <si>
+    <t>1,728.00</t>
+  </si>
+  <si>
+    <t>0.06</t>
+  </si>
+  <si>
+    <t>HLE Glascoat</t>
+  </si>
+  <si>
+    <t>3,403.90</t>
+  </si>
+  <si>
+    <t>66.05</t>
+  </si>
+  <si>
+    <t>1.98</t>
+  </si>
+  <si>
+    <t>Shreyas Shippin</t>
+  </si>
+  <si>
+    <t>262.50</t>
+  </si>
+  <si>
+    <t>12.50</t>
+  </si>
+  <si>
+    <t>21st Cen Mgt</t>
+  </si>
+  <si>
+    <t>28.85</t>
+  </si>
+  <si>
+    <t>Tata Elxsi</t>
+  </si>
+  <si>
+    <t>4,722.20</t>
+  </si>
+  <si>
+    <t>6.95</t>
+  </si>
+  <si>
+    <t>0.15</t>
+  </si>
+  <si>
+    <t>VST Tillers</t>
+  </si>
+  <si>
+    <t>2,621.45</t>
+  </si>
+  <si>
+    <t>405.65</t>
+  </si>
+  <si>
+    <t>18.31</t>
+  </si>
+  <si>
+    <t>6,156.55</t>
+  </si>
+  <si>
+    <t>387.55</t>
+  </si>
+  <si>
+    <t>6.29</t>
+  </si>
+  <si>
+    <t>667,932</t>
+  </si>
+  <si>
+    <t>3,579.55</t>
+  </si>
+  <si>
+    <t>141.20</t>
+  </si>
+  <si>
+    <t>3.94</t>
+  </si>
+  <si>
+    <t>323,144</t>
+  </si>
+  <si>
+    <t>562.95</t>
+  </si>
+  <si>
+    <t>34.50</t>
+  </si>
+  <si>
+    <t>177,755</t>
+  </si>
+  <si>
+    <t>236.50</t>
+  </si>
+  <si>
+    <t>31.25</t>
+  </si>
+  <si>
+    <t>13.21</t>
+  </si>
+  <si>
+    <t>985,820</t>
+  </si>
+  <si>
+    <t>755.35</t>
+  </si>
+  <si>
+    <t>260.30</t>
+  </si>
+  <si>
+    <t>34.46</t>
+  </si>
+  <si>
+    <t>28,728</t>
+  </si>
+  <si>
+    <t>2,939.55</t>
+  </si>
+  <si>
+    <t>56.35</t>
+  </si>
+  <si>
+    <t>1.92</t>
+  </si>
+  <si>
+    <t>113,956</t>
+  </si>
+  <si>
+    <t>671.40</t>
+  </si>
+  <si>
+    <t>9.30</t>
+  </si>
+  <si>
+    <t>1,062,164</t>
+  </si>
+  <si>
+    <t>64.80</t>
+  </si>
+  <si>
+    <t>81,527</t>
+  </si>
+  <si>
+    <t>666.55</t>
+  </si>
+  <si>
+    <t>42.95</t>
+  </si>
+  <si>
+    <t>6.44</t>
+  </si>
+  <si>
+    <t>233,853</t>
+  </si>
+  <si>
+    <t>141.60</t>
+  </si>
+  <si>
+    <t>2.45</t>
+  </si>
+  <si>
+    <t>1.73</t>
+  </si>
+  <si>
+    <t>7,551</t>
+  </si>
+  <si>
+    <t>175.45</t>
+  </si>
+  <si>
+    <t>18.95</t>
+  </si>
+  <si>
+    <t>10.80</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>18,269.55</t>
+  </si>
+  <si>
+    <t>641.45</t>
+  </si>
+  <si>
+    <t>3.51</t>
+  </si>
+  <si>
+    <t>41,123</t>
+  </si>
+  <si>
+    <t>806.60</t>
+  </si>
+  <si>
+    <t>45.95</t>
+  </si>
+  <si>
+    <t>5.70</t>
+  </si>
+  <si>
+    <t>36,108</t>
+  </si>
+  <si>
+    <t>1,720.00</t>
+  </si>
+  <si>
+    <t>8.00</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>3,147.40</t>
+  </si>
+  <si>
+    <t>256.50</t>
+  </si>
+  <si>
+    <t>8.15</t>
+  </si>
+  <si>
+    <t>5,482</t>
+  </si>
+  <si>
+    <t>226.80</t>
+  </si>
+  <si>
+    <t>35.70</t>
+  </si>
+  <si>
+    <t>12,687</t>
+  </si>
+  <si>
+    <t>27.25</t>
+  </si>
+  <si>
+    <t>1.60</t>
+  </si>
+  <si>
+    <t>5.87</t>
+  </si>
+  <si>
+    <t>1,113</t>
+  </si>
+  <si>
+    <t>4,329.10</t>
+  </si>
+  <si>
+    <t>393.10</t>
+  </si>
+  <si>
+    <t>9.08</t>
+  </si>
+  <si>
+    <t>186,542</t>
+  </si>
+  <si>
+    <t>1,897.65</t>
+  </si>
+  <si>
+    <t>723.80</t>
+  </si>
+  <si>
+    <t>38.14</t>
+  </si>
+  <si>
+    <t>15,591</t>
+  </si>
+  <si>
+    <t>18.50</t>
+  </si>
+  <si>
+    <t>15.41</t>
+  </si>
+  <si>
+    <t>4,000</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>LTP</t>
+  </si>
+  <si>
+    <t>Change %</t>
+  </si>
+  <si>
+    <t>Volume (day)</t>
+  </si>
+  <si>
+    <t>Avg volume (Week)</t>
+  </si>
+  <si>
+    <t>Vakrangee Ltd.</t>
+  </si>
+  <si>
+    <t>40.5</t>
+  </si>
+  <si>
+    <t>3.30 (8.9 %)</t>
+  </si>
+  <si>
+    <t>29.6M</t>
+  </si>
+  <si>
+    <t>13.0M</t>
+  </si>
+  <si>
+    <t>Bombay Burmah Tradin..</t>
+  </si>
+  <si>
+    <t>1180.8</t>
+  </si>
+  <si>
+    <t>84.45 (7.7 %)</t>
+  </si>
+  <si>
+    <t>893.1K</t>
+  </si>
+  <si>
+    <t>278.8K</t>
+  </si>
+  <si>
+    <t>Hindustan Unilever L..</t>
+  </si>
+  <si>
+    <t>2619.4</t>
+  </si>
+  <si>
+    <t>133.35 (5.4 %)</t>
+  </si>
+  <si>
+    <t>5.8M</t>
+  </si>
+  <si>
+    <t>2.6M</t>
+  </si>
+  <si>
+    <t>Infibeam Avenues Ltd.</t>
+  </si>
+  <si>
+    <t>42.5</t>
+  </si>
+  <si>
+    <t>2.00 (4.9 %)</t>
+  </si>
+  <si>
+    <t>6.3M</t>
+  </si>
+  <si>
+    <t>3.0M</t>
+  </si>
+  <si>
+    <t>Shilpa Medicare Ltd.</t>
+  </si>
+  <si>
+    <t>573.9</t>
+  </si>
+  <si>
+    <t>26.50 (4.8 %)</t>
+  </si>
+  <si>
+    <t>5.2M</t>
+  </si>
+  <si>
+    <t>1.7M</t>
+  </si>
+  <si>
+    <t>Britannia Industries..</t>
+  </si>
+  <si>
+    <t>3896.0</t>
+  </si>
+  <si>
+    <t>175.20 (4.7 %)</t>
+  </si>
+  <si>
+    <t>1.6M</t>
+  </si>
+  <si>
+    <t>730.6K</t>
+  </si>
+  <si>
+    <t>MindTree Ltd.</t>
+  </si>
+  <si>
+    <t>3345.1</t>
+  </si>
+  <si>
+    <t>148.75 (4.7 %)</t>
+  </si>
+  <si>
+    <t>4.1M</t>
+  </si>
+  <si>
+    <t>2.3M</t>
+  </si>
+  <si>
+    <t>Adani Transmission L..</t>
+  </si>
+  <si>
+    <t>1123.5</t>
+  </si>
+  <si>
+    <t>48.25 (4.5 %)</t>
+  </si>
+  <si>
+    <t>230.8K</t>
+  </si>
+  <si>
+    <t>136.7K</t>
+  </si>
+  <si>
+    <t>Polyplex Corporation..</t>
+  </si>
+  <si>
+    <t>1490.8</t>
+  </si>
+  <si>
+    <t>56.40 (3.9 %)</t>
+  </si>
+  <si>
+    <t>417.0K</t>
+  </si>
+  <si>
+    <t>221.3K</t>
+  </si>
+  <si>
+    <t>Asian Paints Ltd.</t>
+  </si>
+  <si>
+    <t>3113.0</t>
+  </si>
+  <si>
+    <t>111.40 (3.7 %)</t>
+  </si>
+  <si>
+    <t>3.9M</t>
+  </si>
+  <si>
+    <t>2.0M</t>
+  </si>
+  <si>
+    <t>Fortis Healthcare Ltd.</t>
+  </si>
+  <si>
+    <t>277.6</t>
+  </si>
+  <si>
+    <t>9.85 (3.7 %)</t>
+  </si>
+  <si>
+    <t>25.9M</t>
+  </si>
+  <si>
+    <t>17.0M</t>
+  </si>
+  <si>
+    <t>Nestle India Ltd.</t>
+  </si>
+  <si>
+    <t>19571.3</t>
+  </si>
+  <si>
+    <t>660.25 (3.5 %)</t>
+  </si>
+  <si>
+    <t>143.1K</t>
+  </si>
+  <si>
+    <t>75816</t>
+  </si>
+  <si>
+    <t>Lux Industries Ltd.</t>
+  </si>
+  <si>
+    <t>4144.8</t>
+  </si>
+  <si>
+    <t>129.45 (3.2 %)</t>
+  </si>
+  <si>
+    <t>138.6K</t>
+  </si>
+  <si>
+    <t>68183</t>
+  </si>
+  <si>
+    <t>Godrej Agrovet Ltd.</t>
+  </si>
+  <si>
+    <t>639.6</t>
+  </si>
+  <si>
+    <t>19.50 (3.1 %)</t>
+  </si>
+  <si>
+    <t>382.6K</t>
+  </si>
+  <si>
+    <t>196.9K</t>
+  </si>
+  <si>
+    <t>Schneider Electric I..</t>
+  </si>
+  <si>
+    <t>120.5</t>
+  </si>
+  <si>
+    <t>3.30 (2.8 %)</t>
+  </si>
+  <si>
+    <t>13.9M</t>
+  </si>
+  <si>
+    <t>3.8M</t>
+  </si>
+  <si>
+    <t>Godrej Consumer Prod..</t>
+  </si>
+  <si>
+    <t>1033.2</t>
+  </si>
+  <si>
+    <t>27.95 (2.8 %)</t>
+  </si>
+  <si>
+    <t>2.7M</t>
+  </si>
+  <si>
+    <t>1.4M</t>
+  </si>
+  <si>
+    <t>Marico Ltd.</t>
+  </si>
+  <si>
+    <t>537.9</t>
+  </si>
+  <si>
+    <t>14.20 (2.7 %)</t>
+  </si>
+  <si>
+    <t>2.5M</t>
+  </si>
+  <si>
+    <t>Mahindra Logistics L..</t>
+  </si>
+  <si>
+    <t>718.3</t>
+  </si>
+  <si>
+    <t>14.90 (2.1 %)</t>
+  </si>
+  <si>
+    <t>572.2K</t>
+  </si>
+  <si>
+    <t>207.5K</t>
+  </si>
+  <si>
+    <t>Sequent Scientific L..</t>
+  </si>
+  <si>
+    <t>245.4</t>
+  </si>
+  <si>
+    <t>4.80 (2.0 %)</t>
+  </si>
+  <si>
+    <t>1.2M</t>
+  </si>
+  <si>
+    <t>Varun Beverages Ltd.</t>
+  </si>
+  <si>
+    <t>806.7</t>
+  </si>
+  <si>
+    <t>15.65 (2.0 %)</t>
+  </si>
+  <si>
+    <t>685.4K</t>
+  </si>
+  <si>
+    <t>Pidilite Industries ..</t>
+  </si>
+  <si>
+    <t>2267.2</t>
+  </si>
+  <si>
+    <t>41.90 (1.9 %)</t>
+  </si>
+  <si>
+    <t>1.0M</t>
+  </si>
+  <si>
+    <t>536.1K</t>
+  </si>
+  <si>
+    <t>KSB Ltd.</t>
+  </si>
+  <si>
+    <t>20.90 (1.8 %)</t>
+  </si>
+  <si>
+    <t>68565</t>
+  </si>
+  <si>
+    <t>38615</t>
+  </si>
+  <si>
+    <t>Petronet LNG Ltd.</t>
+  </si>
+  <si>
+    <t>226.9</t>
+  </si>
+  <si>
+    <t>3.25 (1.5 %)</t>
+  </si>
+  <si>
+    <t>15.5M</t>
+  </si>
+  <si>
+    <t>9.4M</t>
+  </si>
+  <si>
+    <t>TTK Prestige Ltd.</t>
+  </si>
+  <si>
+    <t>8956.5</t>
+  </si>
+  <si>
+    <t>60.55 (0.7 %)</t>
+  </si>
+  <si>
+    <t>11279</t>
+  </si>
+  <si>
+    <t>6714</t>
+  </si>
+  <si>
+    <t>Berger Paints (India..</t>
+  </si>
+  <si>
+    <t>819.3</t>
+  </si>
+  <si>
+    <t>5.55 (0.7 %)</t>
+  </si>
+  <si>
+    <t>2.8M</t>
+  </si>
+  <si>
+    <t>Chambal Fertilisers ..</t>
+  </si>
+  <si>
+    <t>337.5</t>
+  </si>
+  <si>
+    <t>1.95 (0.6 %)</t>
+  </si>
+  <si>
+    <t>Jindal Saw Ltd.</t>
+  </si>
+  <si>
+    <t>121.7</t>
+  </si>
+  <si>
+    <t>0.70 (0.6 %)</t>
+  </si>
+  <si>
+    <t>2.4M</t>
+  </si>
+  <si>
+    <t>Hindustan Aeronautic..</t>
+  </si>
+  <si>
+    <t>1126.5</t>
+  </si>
+  <si>
+    <t>6.35 (0.6 %)</t>
+  </si>
+  <si>
+    <t>754.7K</t>
+  </si>
+  <si>
+    <t>SKF India Ltd.</t>
+  </si>
+  <si>
+    <t>2766.1</t>
+  </si>
+  <si>
+    <t>12.40 (0.5 %)</t>
+  </si>
+  <si>
+    <t>23606</t>
+  </si>
+  <si>
+    <t>14284</t>
+  </si>
+  <si>
+    <t>Indus Towers Ltd.</t>
+  </si>
+  <si>
+    <t>219.5</t>
+  </si>
+  <si>
+    <t>0.90 (0.4 %)</t>
+  </si>
+  <si>
+    <t>3.5M</t>
+  </si>
+  <si>
+    <t>Zydus Wellness Ltd.</t>
+  </si>
+  <si>
+    <t>2187.6</t>
+  </si>
+  <si>
+    <t>3.10 (0.1 %)</t>
+  </si>
+  <si>
+    <t>64590</t>
+  </si>
+  <si>
+    <t>37376</t>
   </si>
 </sst>
 </file>
@@ -1624,763 +3044,792 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>840</v>
+      </c>
+      <c r="B2" t="s">
+        <v>841</v>
+      </c>
+      <c r="C2" t="s">
+        <v>842</v>
+      </c>
+      <c r="D2" t="s">
+        <v>843</v>
+      </c>
+      <c r="E2" t="s">
+        <v>844</v>
+      </c>
+    </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>309</v>
+        <v>845</v>
       </c>
       <c r="B3" t="s">
-        <v>310</v>
+        <v>846</v>
       </c>
       <c r="C3" t="s">
-        <v>311</v>
+        <v>847</v>
       </c>
       <c r="D3" t="s">
-        <v>312</v>
+        <v>848</v>
       </c>
       <c r="E3" t="s">
-        <v>405</v>
+        <v>849</v>
       </c>
       <c r="F3" t="s">
-        <v>406</v>
+        <v>763</v>
       </c>
       <c r="G3" t="s">
-        <v>76</v>
+        <v>764</v>
       </c>
       <c r="H3" t="s">
-        <v>407</v>
+        <v>765</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>850</v>
       </c>
       <c r="B4" t="s">
-        <v>313</v>
+        <v>851</v>
       </c>
       <c r="C4" t="s">
-        <v>314</v>
+        <v>852</v>
       </c>
       <c r="D4" t="s">
-        <v>315</v>
+        <v>853</v>
       </c>
       <c r="E4" t="s">
-        <v>408</v>
+        <v>854</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>767</v>
       </c>
       <c r="G4" t="s">
-        <v>122</v>
+        <v>768</v>
       </c>
       <c r="H4" t="s">
-        <v>409</v>
+        <v>769</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>316</v>
+        <v>855</v>
       </c>
       <c r="B5" t="s">
-        <v>317</v>
+        <v>856</v>
       </c>
       <c r="C5" t="s">
-        <v>318</v>
+        <v>857</v>
       </c>
       <c r="D5" t="s">
-        <v>319</v>
+        <v>858</v>
       </c>
       <c r="E5" t="s">
-        <v>410</v>
+        <v>859</v>
       </c>
       <c r="F5" t="s">
-        <v>411</v>
+        <v>771</v>
       </c>
       <c r="G5" t="s">
-        <v>412</v>
+        <v>660</v>
       </c>
       <c r="H5" t="s">
-        <v>413</v>
+        <v>772</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>320</v>
+        <v>860</v>
       </c>
       <c r="B6" t="s">
-        <v>321</v>
+        <v>861</v>
       </c>
       <c r="C6" t="s">
-        <v>322</v>
+        <v>862</v>
       </c>
       <c r="D6" t="s">
-        <v>323</v>
+        <v>863</v>
       </c>
       <c r="E6" t="s">
-        <v>414</v>
+        <v>864</v>
       </c>
       <c r="F6" t="s">
-        <v>415</v>
+        <v>774</v>
       </c>
       <c r="G6" t="s">
-        <v>251</v>
+        <v>775</v>
       </c>
       <c r="H6" t="s">
-        <v>416</v>
+        <v>776</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>865</v>
       </c>
       <c r="B7" t="s">
-        <v>324</v>
+        <v>866</v>
       </c>
       <c r="C7" t="s">
-        <v>325</v>
+        <v>867</v>
       </c>
       <c r="D7" t="s">
-        <v>326</v>
+        <v>868</v>
       </c>
       <c r="E7" t="s">
-        <v>417</v>
+        <v>869</v>
       </c>
       <c r="F7" t="s">
-        <v>322</v>
+        <v>778</v>
       </c>
       <c r="G7" t="s">
-        <v>418</v>
+        <v>779</v>
       </c>
       <c r="H7" t="s">
-        <v>419</v>
+        <v>780</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>870</v>
       </c>
       <c r="B8" t="s">
-        <v>327</v>
+        <v>871</v>
       </c>
       <c r="C8" t="s">
-        <v>328</v>
+        <v>872</v>
       </c>
       <c r="D8" t="s">
-        <v>329</v>
+        <v>873</v>
       </c>
       <c r="E8" t="s">
-        <v>420</v>
+        <v>874</v>
       </c>
       <c r="F8" t="s">
-        <v>421</v>
+        <v>782</v>
       </c>
       <c r="G8" t="s">
-        <v>422</v>
+        <v>783</v>
       </c>
       <c r="H8" t="s">
-        <v>423</v>
+        <v>784</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>330</v>
+        <v>875</v>
       </c>
       <c r="B9" t="s">
-        <v>331</v>
+        <v>876</v>
       </c>
       <c r="C9" t="s">
-        <v>332</v>
+        <v>877</v>
       </c>
       <c r="D9" t="s">
+        <v>878</v>
+      </c>
+      <c r="E9" t="s">
+        <v>879</v>
+      </c>
+      <c r="F9" t="s">
+        <v>786</v>
+      </c>
+      <c r="G9" t="s">
         <v>333</v>
       </c>
-      <c r="E9" t="s">
-        <v>424</v>
-      </c>
-      <c r="F9" t="s">
-        <v>425</v>
-      </c>
-      <c r="G9" t="s">
-        <v>426</v>
-      </c>
       <c r="H9" t="s">
-        <v>427</v>
+        <v>787</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>334</v>
+        <v>880</v>
       </c>
       <c r="B10" t="s">
-        <v>169</v>
+        <v>881</v>
       </c>
       <c r="C10" t="s">
-        <v>335</v>
+        <v>882</v>
       </c>
       <c r="D10" t="s">
-        <v>336</v>
+        <v>883</v>
       </c>
       <c r="E10" t="s">
-        <v>428</v>
+        <v>884</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
+        <v>585</v>
       </c>
       <c r="G10" t="s">
-        <v>429</v>
+        <v>530</v>
       </c>
       <c r="H10" t="s">
-        <v>430</v>
+        <v>789</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>885</v>
       </c>
       <c r="B11" t="s">
-        <v>337</v>
+        <v>886</v>
       </c>
       <c r="C11" t="s">
-        <v>338</v>
+        <v>887</v>
       </c>
       <c r="D11" t="s">
-        <v>339</v>
+        <v>888</v>
       </c>
       <c r="E11" t="s">
-        <v>431</v>
+        <v>889</v>
       </c>
       <c r="F11" t="s">
-        <v>432</v>
+        <v>791</v>
       </c>
       <c r="G11" t="s">
-        <v>433</v>
+        <v>792</v>
       </c>
       <c r="H11" t="s">
-        <v>434</v>
+        <v>793</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>340</v>
+        <v>890</v>
       </c>
       <c r="B12" t="s">
-        <v>341</v>
+        <v>891</v>
       </c>
       <c r="C12" t="s">
-        <v>342</v>
+        <v>892</v>
       </c>
       <c r="D12" t="s">
-        <v>343</v>
+        <v>893</v>
       </c>
       <c r="E12" t="s">
-        <v>435</v>
+        <v>894</v>
       </c>
       <c r="F12" t="s">
-        <v>436</v>
+        <v>795</v>
       </c>
       <c r="G12" t="s">
-        <v>437</v>
+        <v>796</v>
       </c>
       <c r="H12" t="s">
-        <v>438</v>
+        <v>797</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>344</v>
+        <v>895</v>
       </c>
       <c r="B13" t="s">
-        <v>345</v>
+        <v>896</v>
       </c>
       <c r="C13" t="s">
-        <v>346</v>
+        <v>897</v>
       </c>
       <c r="D13" t="s">
-        <v>347</v>
+        <v>898</v>
       </c>
       <c r="E13" t="s">
-        <v>439</v>
+        <v>899</v>
       </c>
       <c r="F13" t="s">
-        <v>440</v>
+        <v>799</v>
       </c>
       <c r="G13" t="s">
-        <v>441</v>
+        <v>800</v>
       </c>
       <c r="H13" t="s">
-        <v>442</v>
+        <v>801</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>900</v>
       </c>
       <c r="B14" t="s">
-        <v>348</v>
+        <v>901</v>
       </c>
       <c r="C14" t="s">
-        <v>349</v>
+        <v>902</v>
       </c>
       <c r="D14" t="s">
-        <v>350</v>
+        <v>903</v>
       </c>
       <c r="E14" t="s">
-        <v>443</v>
+        <v>904</v>
       </c>
       <c r="F14" t="s">
-        <v>444</v>
+        <v>803</v>
       </c>
       <c r="G14" t="s">
-        <v>445</v>
+        <v>804</v>
       </c>
       <c r="H14" t="s">
-        <v>446</v>
+        <v>805</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>351</v>
+        <v>905</v>
       </c>
       <c r="B15" t="s">
-        <v>352</v>
+        <v>906</v>
       </c>
       <c r="C15" t="s">
-        <v>353</v>
+        <v>907</v>
       </c>
       <c r="D15" t="s">
-        <v>354</v>
+        <v>908</v>
       </c>
       <c r="E15" t="s">
-        <v>447</v>
+        <v>909</v>
       </c>
       <c r="F15" t="s">
-        <v>448</v>
+        <v>807</v>
       </c>
       <c r="G15" t="s">
-        <v>449</v>
+        <v>808</v>
       </c>
       <c r="H15" t="s">
-        <v>450</v>
+        <v>809</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>355</v>
+        <v>910</v>
       </c>
       <c r="B16" t="s">
-        <v>356</v>
+        <v>911</v>
       </c>
       <c r="C16" t="s">
-        <v>357</v>
+        <v>912</v>
       </c>
       <c r="D16" t="s">
-        <v>358</v>
+        <v>913</v>
       </c>
       <c r="E16" t="s">
-        <v>451</v>
+        <v>914</v>
       </c>
       <c r="F16" t="s">
-        <v>397</v>
+        <v>811</v>
       </c>
       <c r="G16" t="s">
-        <v>452</v>
+        <v>387</v>
       </c>
       <c r="H16" t="s">
-        <v>453</v>
+        <v>812</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>359</v>
+        <v>915</v>
       </c>
       <c r="B17" t="s">
-        <v>360</v>
+        <v>916</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>917</v>
       </c>
       <c r="D17" t="s">
-        <v>361</v>
+        <v>918</v>
       </c>
       <c r="E17" t="s">
-        <v>454</v>
+        <v>919</v>
       </c>
       <c r="F17" t="s">
-        <v>455</v>
+        <v>814</v>
       </c>
       <c r="G17" t="s">
-        <v>456</v>
+        <v>815</v>
       </c>
       <c r="H17" t="s">
-        <v>457</v>
+        <v>816</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>920</v>
       </c>
       <c r="B18" t="s">
-        <v>362</v>
+        <v>921</v>
       </c>
       <c r="C18" t="s">
-        <v>363</v>
+        <v>922</v>
       </c>
       <c r="D18" t="s">
-        <v>364</v>
+        <v>863</v>
       </c>
       <c r="E18" t="s">
-        <v>458</v>
+        <v>923</v>
       </c>
       <c r="F18" t="s">
-        <v>459</v>
+        <v>818</v>
       </c>
       <c r="G18" t="s">
-        <v>460</v>
+        <v>558</v>
       </c>
       <c r="H18" t="s">
-        <v>461</v>
+        <v>819</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>924</v>
       </c>
       <c r="B19" t="s">
-        <v>365</v>
+        <v>925</v>
       </c>
       <c r="C19" t="s">
-        <v>239</v>
+        <v>926</v>
       </c>
       <c r="D19" t="s">
-        <v>366</v>
+        <v>927</v>
       </c>
       <c r="E19" t="s">
-        <v>462</v>
+        <v>928</v>
       </c>
       <c r="F19" t="s">
-        <v>463</v>
+        <v>821</v>
       </c>
       <c r="G19" t="s">
-        <v>205</v>
+        <v>822</v>
       </c>
       <c r="H19" t="s">
-        <v>464</v>
+        <v>823</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>367</v>
+        <v>929</v>
       </c>
       <c r="B20" t="s">
-        <v>368</v>
+        <v>930</v>
       </c>
       <c r="C20" t="s">
-        <v>369</v>
+        <v>931</v>
       </c>
       <c r="D20" t="s">
-        <v>370</v>
+        <v>889</v>
       </c>
       <c r="E20" t="s">
-        <v>465</v>
+        <v>932</v>
       </c>
       <c r="F20" t="s">
-        <v>466</v>
+        <v>825</v>
       </c>
       <c r="G20" t="s">
-        <v>467</v>
+        <v>826</v>
       </c>
       <c r="H20" t="s">
-        <v>468</v>
+        <v>827</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>371</v>
+        <v>933</v>
       </c>
       <c r="B21" t="s">
-        <v>372</v>
+        <v>934</v>
       </c>
       <c r="C21" t="s">
-        <v>261</v>
+        <v>935</v>
       </c>
       <c r="D21" t="s">
-        <v>373</v>
+        <v>932</v>
       </c>
       <c r="E21" t="s">
-        <v>469</v>
+        <v>936</v>
       </c>
       <c r="F21" t="s">
-        <v>470</v>
+        <v>829</v>
       </c>
       <c r="G21" t="s">
-        <v>471</v>
+        <v>830</v>
       </c>
       <c r="H21" t="s">
-        <v>472</v>
+        <v>831</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>937</v>
       </c>
       <c r="B22" t="s">
-        <v>374</v>
+        <v>938</v>
       </c>
       <c r="C22" t="s">
-        <v>258</v>
+        <v>939</v>
       </c>
       <c r="D22" t="s">
-        <v>299</v>
+        <v>940</v>
       </c>
       <c r="E22" t="s">
-        <v>473</v>
+        <v>941</v>
       </c>
       <c r="F22" t="s">
-        <v>325</v>
+        <v>227</v>
       </c>
       <c r="G22" t="s">
-        <v>474</v>
+        <v>833</v>
       </c>
       <c r="H22" t="s">
-        <v>475</v>
+        <v>834</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>375</v>
+        <v>942</v>
       </c>
       <c r="B23" t="s">
-        <v>376</v>
+        <v>846</v>
       </c>
       <c r="C23" t="s">
-        <v>377</v>
+        <v>943</v>
       </c>
       <c r="D23" t="s">
-        <v>378</v>
+        <v>944</v>
       </c>
       <c r="E23" t="s">
-        <v>476</v>
+        <v>945</v>
       </c>
       <c r="F23" t="s">
-        <v>477</v>
+        <v>670</v>
       </c>
       <c r="G23" t="s">
-        <v>478</v>
+        <v>671</v>
       </c>
       <c r="H23" t="s">
-        <v>479</v>
+        <v>672</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>946</v>
       </c>
       <c r="B24" t="s">
-        <v>379</v>
+        <v>947</v>
       </c>
       <c r="C24" t="s">
-        <v>380</v>
+        <v>948</v>
       </c>
       <c r="D24" t="s">
-        <v>99</v>
+        <v>949</v>
       </c>
       <c r="E24" t="s">
-        <v>480</v>
+        <v>950</v>
       </c>
       <c r="F24" t="s">
-        <v>481</v>
+        <v>599</v>
       </c>
       <c r="G24" t="s">
-        <v>482</v>
+        <v>674</v>
       </c>
       <c r="H24" t="s">
-        <v>483</v>
+        <v>675</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>951</v>
       </c>
       <c r="B25" t="s">
-        <v>381</v>
+        <v>952</v>
       </c>
       <c r="C25" t="s">
-        <v>382</v>
+        <v>953</v>
       </c>
       <c r="D25" t="s">
-        <v>383</v>
+        <v>954</v>
       </c>
       <c r="E25" t="s">
-        <v>377</v>
+        <v>955</v>
       </c>
       <c r="F25" t="s">
-        <v>484</v>
+        <v>676</v>
       </c>
       <c r="G25" t="s">
-        <v>485</v>
+        <v>640</v>
       </c>
       <c r="H25" t="s">
-        <v>191</v>
+        <v>677</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>384</v>
+        <v>956</v>
       </c>
       <c r="B26" t="s">
-        <v>385</v>
+        <v>957</v>
       </c>
       <c r="C26" t="s">
-        <v>386</v>
+        <v>958</v>
       </c>
       <c r="D26" t="s">
-        <v>387</v>
+        <v>959</v>
       </c>
       <c r="E26" t="s">
-        <v>486</v>
+        <v>932</v>
       </c>
       <c r="F26" t="s">
-        <v>487</v>
+        <v>31</v>
       </c>
       <c r="G26" t="s">
-        <v>488</v>
+        <v>679</v>
       </c>
       <c r="H26" t="s">
-        <v>489</v>
+        <v>680</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>92</v>
+        <v>960</v>
       </c>
       <c r="B27" t="s">
-        <v>388</v>
+        <v>961</v>
       </c>
       <c r="C27" t="s">
-        <v>389</v>
+        <v>962</v>
       </c>
       <c r="D27" t="s">
-        <v>390</v>
+        <v>854</v>
       </c>
       <c r="E27" t="s">
-        <v>490</v>
+        <v>864</v>
       </c>
       <c r="F27" t="s">
-        <v>491</v>
+        <v>682</v>
       </c>
       <c r="G27" t="s">
-        <v>492</v>
+        <v>683</v>
       </c>
       <c r="H27" t="s">
-        <v>493</v>
+        <v>684</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>391</v>
+        <v>963</v>
       </c>
       <c r="B28" t="s">
-        <v>392</v>
+        <v>964</v>
       </c>
       <c r="C28" t="s">
-        <v>393</v>
+        <v>965</v>
       </c>
       <c r="D28" t="s">
-        <v>394</v>
+        <v>888</v>
       </c>
       <c r="E28" t="s">
-        <v>494</v>
+        <v>966</v>
       </c>
       <c r="F28" t="s">
-        <v>389</v>
+        <v>686</v>
       </c>
       <c r="G28" t="s">
-        <v>495</v>
+        <v>687</v>
       </c>
       <c r="H28" t="s">
-        <v>496</v>
+        <v>688</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>395</v>
+        <v>967</v>
       </c>
       <c r="B29" t="s">
-        <v>396</v>
+        <v>968</v>
       </c>
       <c r="C29" t="s">
-        <v>397</v>
+        <v>969</v>
       </c>
       <c r="D29" t="s">
-        <v>47</v>
+        <v>864</v>
       </c>
       <c r="E29" t="s">
-        <v>497</v>
+        <v>970</v>
       </c>
       <c r="F29" t="s">
-        <v>232</v>
+        <v>335</v>
       </c>
       <c r="G29" t="s">
-        <v>498</v>
+        <v>689</v>
       </c>
       <c r="H29" t="s">
-        <v>499</v>
+        <v>690</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>398</v>
+        <v>971</v>
       </c>
       <c r="B30" t="s">
-        <v>399</v>
+        <v>972</v>
       </c>
       <c r="C30" t="s">
-        <v>400</v>
+        <v>973</v>
       </c>
       <c r="D30" t="s">
-        <v>401</v>
+        <v>974</v>
       </c>
       <c r="E30" t="s">
-        <v>500</v>
+        <v>975</v>
       </c>
       <c r="F30" t="s">
-        <v>501</v>
+        <v>692</v>
       </c>
       <c r="G30" t="s">
-        <v>502</v>
+        <v>693</v>
       </c>
       <c r="H30" t="s">
-        <v>503</v>
+        <v>694</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>402</v>
+        <v>976</v>
       </c>
       <c r="B31" t="s">
-        <v>403</v>
+        <v>977</v>
       </c>
       <c r="C31" t="s">
-        <v>404</v>
+        <v>978</v>
       </c>
       <c r="D31" t="s">
-        <v>347</v>
+        <v>853</v>
       </c>
       <c r="E31" t="s">
-        <v>504</v>
+        <v>979</v>
       </c>
       <c r="F31" t="s">
-        <v>505</v>
+        <v>696</v>
       </c>
       <c r="G31" t="s">
-        <v>506</v>
+        <v>697</v>
       </c>
       <c r="H31" t="s">
-        <v>507</v>
+        <v>698</v>
       </c>
     </row>
     <row r="32">
+      <c r="A32" t="s">
+        <v>980</v>
+      </c>
+      <c r="B32" t="s">
+        <v>981</v>
+      </c>
+      <c r="C32" t="s">
+        <v>982</v>
+      </c>
+      <c r="D32" t="s">
+        <v>983</v>
+      </c>
       <c r="E32" t="s">
-        <v>508</v>
+        <v>984</v>
       </c>
       <c r="F32" t="s">
         <v>509</v>
@@ -2390,6 +3839,36 @@
       </c>
       <c r="H32" t="s">
         <v>511</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>835</v>
+      </c>
+      <c r="B1" t="s">
+        <v>836</v>
+      </c>
+      <c r="C1" t="s">
+        <v>837</v>
+      </c>
+      <c r="D1" t="s">
+        <v>838</v>
+      </c>
+      <c r="E1" t="s">
+        <v>839</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in trendlyn commit
</commit_message>
<xml_diff>
--- a/Reports/test.xlsx
+++ b/Reports/test.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="985">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="1305">
   <si>
     <t>Company</t>
   </si>
@@ -2968,6 +2968,966 @@
   </si>
   <si>
     <t>37376</t>
+  </si>
+  <si>
+    <t>InterGlobe Aviation ..</t>
+  </si>
+  <si>
+    <t>2196.1</t>
+  </si>
+  <si>
+    <t>216.20 (10.9 %)</t>
+  </si>
+  <si>
+    <t>8.4M</t>
+  </si>
+  <si>
+    <t>Karur Vysya Bank Ltd.</t>
+  </si>
+  <si>
+    <t>49.9</t>
+  </si>
+  <si>
+    <t>4.25 (9.3 %)</t>
+  </si>
+  <si>
+    <t>41.3M</t>
+  </si>
+  <si>
+    <t>10.5M</t>
+  </si>
+  <si>
+    <t>Tata Elxsi Ltd.</t>
+  </si>
+  <si>
+    <t>5490.7</t>
+  </si>
+  <si>
+    <t>337.05 (6.5 %)</t>
+  </si>
+  <si>
+    <t>577.4K</t>
+  </si>
+  <si>
+    <t>311.3K</t>
+  </si>
+  <si>
+    <t>DCM Shriram Ltd.</t>
+  </si>
+  <si>
+    <t>1036.8</t>
+  </si>
+  <si>
+    <t>58.70 (6.0 %)</t>
+  </si>
+  <si>
+    <t>403.5K</t>
+  </si>
+  <si>
+    <t>154.2K</t>
+  </si>
+  <si>
+    <t>Venky's (India) Ltd.</t>
+  </si>
+  <si>
+    <t>3060.0</t>
+  </si>
+  <si>
+    <t>165.60 (5.7 %)</t>
+  </si>
+  <si>
+    <t>470.2K</t>
+  </si>
+  <si>
+    <t>163.9K</t>
+  </si>
+  <si>
+    <t>Himadri Speciality C..</t>
+  </si>
+  <si>
+    <t>50.1</t>
+  </si>
+  <si>
+    <t>2.65 (5.6 %)</t>
+  </si>
+  <si>
+    <t>19.0M</t>
+  </si>
+  <si>
+    <t>6.0M</t>
+  </si>
+  <si>
+    <t>Kotak Mahindra Bank ..</t>
+  </si>
+  <si>
+    <t>2008.0</t>
+  </si>
+  <si>
+    <t>101.15 (5.3 %)</t>
+  </si>
+  <si>
+    <t>14.6M</t>
+  </si>
+  <si>
+    <t>6.2M</t>
+  </si>
+  <si>
+    <t>Jamna Auto Industrie..</t>
+  </si>
+  <si>
+    <t>96.5</t>
+  </si>
+  <si>
+    <t>4.25 (4.6 %)</t>
+  </si>
+  <si>
+    <t>10.3M</t>
+  </si>
+  <si>
+    <t>Motilal Oswal Financ..</t>
+  </si>
+  <si>
+    <t>818.3</t>
+  </si>
+  <si>
+    <t>33.15 (4.2 %)</t>
+  </si>
+  <si>
+    <t>565.2K</t>
+  </si>
+  <si>
+    <t>IFB Industries Ltd.</t>
+  </si>
+  <si>
+    <t>1210.0</t>
+  </si>
+  <si>
+    <t>46.70 (4.0 %)</t>
+  </si>
+  <si>
+    <t>259.5K</t>
+  </si>
+  <si>
+    <t>170.8K</t>
+  </si>
+  <si>
+    <t>PNB Housing Finance ..</t>
+  </si>
+  <si>
+    <t>660.7</t>
+  </si>
+  <si>
+    <t>25.15 (4.0 %)</t>
+  </si>
+  <si>
+    <t>179.0K</t>
+  </si>
+  <si>
+    <t>104.1K</t>
+  </si>
+  <si>
+    <t>Mahindra CIE Automot..</t>
+  </si>
+  <si>
+    <t>236.0</t>
+  </si>
+  <si>
+    <t>8.95 (3.9 %)</t>
+  </si>
+  <si>
+    <t>924.5K</t>
+  </si>
+  <si>
+    <t>319.3K</t>
+  </si>
+  <si>
+    <t>JSW Energy Ltd.</t>
+  </si>
+  <si>
+    <t>323.5</t>
+  </si>
+  <si>
+    <t>12.10 (3.9 %)</t>
+  </si>
+  <si>
+    <t>5.7M</t>
+  </si>
+  <si>
+    <t>Avenue Supermarts Ltd.</t>
+  </si>
+  <si>
+    <t>4239.7</t>
+  </si>
+  <si>
+    <t>155.15 (3.8 %)</t>
+  </si>
+  <si>
+    <t>767.5K</t>
+  </si>
+  <si>
+    <t>388.7K</t>
+  </si>
+  <si>
+    <t>Ingersoll-Rand (Indi..</t>
+  </si>
+  <si>
+    <t>998.5</t>
+  </si>
+  <si>
+    <t>34.75 (3.6 %)</t>
+  </si>
+  <si>
+    <t>182.2K</t>
+  </si>
+  <si>
+    <t>66082</t>
+  </si>
+  <si>
+    <t>1244.6</t>
+  </si>
+  <si>
+    <t>43.35 (3.6 %)</t>
+  </si>
+  <si>
+    <t>551.8K</t>
+  </si>
+  <si>
+    <t>126.2K</t>
+  </si>
+  <si>
+    <t>Gujarat Ambuja Expor..</t>
+  </si>
+  <si>
+    <t>181.6</t>
+  </si>
+  <si>
+    <t>6.10 (3.5 %)</t>
+  </si>
+  <si>
+    <t>631.4K</t>
+  </si>
+  <si>
+    <t>312.7K</t>
+  </si>
+  <si>
+    <t>Spicejet Ltd.</t>
+  </si>
+  <si>
+    <t>78.6</t>
+  </si>
+  <si>
+    <t>2.60 (3.4 %)</t>
+  </si>
+  <si>
+    <t>33.2M</t>
+  </si>
+  <si>
+    <t>Bajaj Electricals Ltd.</t>
+  </si>
+  <si>
+    <t>48.10 (3.3 %)</t>
+  </si>
+  <si>
+    <t>1.9M</t>
+  </si>
+  <si>
+    <t>618.2K</t>
+  </si>
+  <si>
+    <t>Mahindra &amp; Mahindra ..</t>
+  </si>
+  <si>
+    <t>179.4</t>
+  </si>
+  <si>
+    <t>5.75 (3.3 %)</t>
+  </si>
+  <si>
+    <t>20.0M</t>
+  </si>
+  <si>
+    <t>8.6M</t>
+  </si>
+  <si>
+    <t>Crisil Ltd.</t>
+  </si>
+  <si>
+    <t>2912.2</t>
+  </si>
+  <si>
+    <t>93.00 (3.3 %)</t>
+  </si>
+  <si>
+    <t>218.1K</t>
+  </si>
+  <si>
+    <t>68656</t>
+  </si>
+  <si>
+    <t>Symphony Ltd.</t>
+  </si>
+  <si>
+    <t>1027.3</t>
+  </si>
+  <si>
+    <t>32.60 (3.3 %)</t>
+  </si>
+  <si>
+    <t>274.2K</t>
+  </si>
+  <si>
+    <t>101.1K</t>
+  </si>
+  <si>
+    <t>Burger King India Ltd.</t>
+  </si>
+  <si>
+    <t>164.7</t>
+  </si>
+  <si>
+    <t>4.45 (2.8 %)</t>
+  </si>
+  <si>
+    <t>5.0M</t>
+  </si>
+  <si>
+    <t>2.1M</t>
+  </si>
+  <si>
+    <t>Polycab India Ltd.</t>
+  </si>
+  <si>
+    <t>2505.8</t>
+  </si>
+  <si>
+    <t>63.45 (2.6 %)</t>
+  </si>
+  <si>
+    <t>2.2M</t>
+  </si>
+  <si>
+    <t>880.1K</t>
+  </si>
+  <si>
+    <t>Westlife Development..</t>
+  </si>
+  <si>
+    <t>543.4</t>
+  </si>
+  <si>
+    <t>12.50 (2.4 %)</t>
+  </si>
+  <si>
+    <t>187.2K</t>
+  </si>
+  <si>
+    <t>92953</t>
+  </si>
+  <si>
+    <t>Vardhman Textiles Ltd.</t>
+  </si>
+  <si>
+    <t>1911.9</t>
+  </si>
+  <si>
+    <t>43.10 (2.3 %)</t>
+  </si>
+  <si>
+    <t>135.9K</t>
+  </si>
+  <si>
+    <t>71547</t>
+  </si>
+  <si>
+    <t>Intellect Design Are..</t>
+  </si>
+  <si>
+    <t>677.6</t>
+  </si>
+  <si>
+    <t>15.30 (2.3 %)</t>
+  </si>
+  <si>
+    <t>825.0K</t>
+  </si>
+  <si>
+    <t>398.4K</t>
+  </si>
+  <si>
+    <t>Housing and Urban De..</t>
+  </si>
+  <si>
+    <t>44.8</t>
+  </si>
+  <si>
+    <t>1.00 (2.3 %)</t>
+  </si>
+  <si>
+    <t>3.6M</t>
+  </si>
+  <si>
+    <t>Dabur India Ltd.</t>
+  </si>
+  <si>
+    <t>654.0</t>
+  </si>
+  <si>
+    <t>13.55 (2.1 %)</t>
+  </si>
+  <si>
+    <t>1.8M</t>
+  </si>
+  <si>
+    <t>KPR Mill Ltd.</t>
+  </si>
+  <si>
+    <t>2222.1</t>
+  </si>
+  <si>
+    <t>45.40 (2.1 %)</t>
+  </si>
+  <si>
+    <t>213.4K</t>
+  </si>
+  <si>
+    <t>139.7K</t>
+  </si>
+  <si>
+    <t>Edelweiss Financial ..</t>
+  </si>
+  <si>
+    <t>83.0</t>
+  </si>
+  <si>
+    <t>1.65 (2.0 %)</t>
+  </si>
+  <si>
+    <t>5.1M</t>
+  </si>
+  <si>
+    <t>Ratnamani Metals &amp; T..</t>
+  </si>
+  <si>
+    <t>2193.9</t>
+  </si>
+  <si>
+    <t>42.00 (2.0 %)</t>
+  </si>
+  <si>
+    <t>151.0K</t>
+  </si>
+  <si>
+    <t>48386</t>
+  </si>
+  <si>
+    <t>Radico Khaitan Ltd.</t>
+  </si>
+  <si>
+    <t>924.9</t>
+  </si>
+  <si>
+    <t>17.65 (2.0 %)</t>
+  </si>
+  <si>
+    <t>645.0K</t>
+  </si>
+  <si>
+    <t>Great Eastern Shippi..</t>
+  </si>
+  <si>
+    <t>376.2</t>
+  </si>
+  <si>
+    <t>7.00 (1.9 %)</t>
+  </si>
+  <si>
+    <t>755.1K</t>
+  </si>
+  <si>
+    <t>Bajaj Holdings &amp; Inv..</t>
+  </si>
+  <si>
+    <t>4398.9</t>
+  </si>
+  <si>
+    <t>79.60 (1.8 %)</t>
+  </si>
+  <si>
+    <t>845.3K</t>
+  </si>
+  <si>
+    <t>186.1K</t>
+  </si>
+  <si>
+    <t>V-Guard Industries L..</t>
+  </si>
+  <si>
+    <t>259.6</t>
+  </si>
+  <si>
+    <t>4.65 (1.8 %)</t>
+  </si>
+  <si>
+    <t>Cera Sanitaryware Ltd.</t>
+  </si>
+  <si>
+    <t>4478.4</t>
+  </si>
+  <si>
+    <t>78.95 (1.8 %)</t>
+  </si>
+  <si>
+    <t>30887</t>
+  </si>
+  <si>
+    <t>16414</t>
+  </si>
+  <si>
+    <t>Century Textiles &amp; I..</t>
+  </si>
+  <si>
+    <t>850.0</t>
+  </si>
+  <si>
+    <t>14.75 (1.8 %)</t>
+  </si>
+  <si>
+    <t>851.3K</t>
+  </si>
+  <si>
+    <t>413.9K</t>
+  </si>
+  <si>
+    <t>Cochin Shipyard Ltd.</t>
+  </si>
+  <si>
+    <t>378.1</t>
+  </si>
+  <si>
+    <t>6.05 (1.6 %)</t>
+  </si>
+  <si>
+    <t>449.2K</t>
+  </si>
+  <si>
+    <t>288.1K</t>
+  </si>
+  <si>
+    <t>Schaeffler India Ltd.</t>
+  </si>
+  <si>
+    <t>7299.9</t>
+  </si>
+  <si>
+    <t>114.25 (1.6 %)</t>
+  </si>
+  <si>
+    <t>15698</t>
+  </si>
+  <si>
+    <t>10198</t>
+  </si>
+  <si>
+    <t>Lakshmi Machine Work..</t>
+  </si>
+  <si>
+    <t>8278.1</t>
+  </si>
+  <si>
+    <t>116.85 (1.4 %)</t>
+  </si>
+  <si>
+    <t>15376</t>
+  </si>
+  <si>
+    <t>9349</t>
+  </si>
+  <si>
+    <t>HDFC Bank Ltd.</t>
+  </si>
+  <si>
+    <t>1582.2</t>
+  </si>
+  <si>
+    <t>22.20 (1.4 %)</t>
+  </si>
+  <si>
+    <t>10.2M</t>
+  </si>
+  <si>
+    <t>6.4M</t>
+  </si>
+  <si>
+    <t>Tata Investment Corp..</t>
+  </si>
+  <si>
+    <t>1301.6</t>
+  </si>
+  <si>
+    <t>17.40 (1.4 %)</t>
+  </si>
+  <si>
+    <t>76725</t>
+  </si>
+  <si>
+    <t>45236</t>
+  </si>
+  <si>
+    <t>Eicher Motors Ltd.</t>
+  </si>
+  <si>
+    <t>2898.6</t>
+  </si>
+  <si>
+    <t>38.35 (1.3 %)</t>
+  </si>
+  <si>
+    <t>663.9K</t>
+  </si>
+  <si>
+    <t>Havells India Ltd.</t>
+  </si>
+  <si>
+    <t>1471.9</t>
+  </si>
+  <si>
+    <t>18.80 (1.3 %)</t>
+  </si>
+  <si>
+    <t>1.3M</t>
+  </si>
+  <si>
+    <t>Mas Financial Servic..</t>
+  </si>
+  <si>
+    <t>794.4</t>
+  </si>
+  <si>
+    <t>9.40 (1.2 %)</t>
+  </si>
+  <si>
+    <t>79465</t>
+  </si>
+  <si>
+    <t>44056</t>
+  </si>
+  <si>
+    <t>Maruti Suzuki India ..</t>
+  </si>
+  <si>
+    <t>7014.5</t>
+  </si>
+  <si>
+    <t>83.50 (1.2 %)</t>
+  </si>
+  <si>
+    <t>980.8K</t>
+  </si>
+  <si>
+    <t>634.7K</t>
+  </si>
+  <si>
+    <t>VIP Industries Ltd.</t>
+  </si>
+  <si>
+    <t>498.8</t>
+  </si>
+  <si>
+    <t>5.80 (1.2 %)</t>
+  </si>
+  <si>
+    <t>SBI Life Insurance C..</t>
+  </si>
+  <si>
+    <t>1198.8</t>
+  </si>
+  <si>
+    <t>13.90 (1.2 %)</t>
+  </si>
+  <si>
+    <t>KEI Industries Ltd.</t>
+  </si>
+  <si>
+    <t>844.2</t>
+  </si>
+  <si>
+    <t>8.70 (1.0 %)</t>
+  </si>
+  <si>
+    <t>3.4M</t>
+  </si>
+  <si>
+    <t>Gulf Oil Lubricants ..</t>
+  </si>
+  <si>
+    <t>615.9</t>
+  </si>
+  <si>
+    <t>6.25 (1.0 %)</t>
+  </si>
+  <si>
+    <t>94710</t>
+  </si>
+  <si>
+    <t>53955</t>
+  </si>
+  <si>
+    <t>Maharashtra Scooters..</t>
+  </si>
+  <si>
+    <t>4431.8</t>
+  </si>
+  <si>
+    <t>40.20 (0.9 %)</t>
+  </si>
+  <si>
+    <t>40334</t>
+  </si>
+  <si>
+    <t>14184</t>
+  </si>
+  <si>
+    <t>J B Chemicals &amp; Phar..</t>
+  </si>
+  <si>
+    <t>1740.7</t>
+  </si>
+  <si>
+    <t>14.70 (0.9 %)</t>
+  </si>
+  <si>
+    <t>219.6K</t>
+  </si>
+  <si>
+    <t>131.9K</t>
+  </si>
+  <si>
+    <t>Solar Industries Ind..</t>
+  </si>
+  <si>
+    <t>1979.1</t>
+  </si>
+  <si>
+    <t>15.85 (0.8 %)</t>
+  </si>
+  <si>
+    <t>616.3K</t>
+  </si>
+  <si>
+    <t>311.2K</t>
+  </si>
+  <si>
+    <t>Star Cement Ltd.</t>
+  </si>
+  <si>
+    <t>108.7</t>
+  </si>
+  <si>
+    <t>0.85 (0.8 %)</t>
+  </si>
+  <si>
+    <t>669.1K</t>
+  </si>
+  <si>
+    <t>351.6K</t>
+  </si>
+  <si>
+    <t>Apollo Tyres Ltd.</t>
+  </si>
+  <si>
+    <t>223.6</t>
+  </si>
+  <si>
+    <t>1.65 (0.7 %)</t>
+  </si>
+  <si>
+    <t>6.9M</t>
+  </si>
+  <si>
+    <t>4.0M</t>
+  </si>
+  <si>
+    <t>20175.7</t>
+  </si>
+  <si>
+    <t>147.85 (0.7 %)</t>
+  </si>
+  <si>
+    <t>95129</t>
+  </si>
+  <si>
+    <t>56137</t>
+  </si>
+  <si>
+    <t>Bajaj Finserv Ltd.</t>
+  </si>
+  <si>
+    <t>16840.2</t>
+  </si>
+  <si>
+    <t>107.20 (0.6 %)</t>
+  </si>
+  <si>
+    <t>655.0K</t>
+  </si>
+  <si>
+    <t>261.6K</t>
+  </si>
+  <si>
+    <t>PNC Infratech Ltd.</t>
+  </si>
+  <si>
+    <t>372.7</t>
+  </si>
+  <si>
+    <t>2.30 (0.6 %)</t>
+  </si>
+  <si>
+    <t>1.1M</t>
+  </si>
+  <si>
+    <t>Axis Bank Ltd.</t>
+  </si>
+  <si>
+    <t>807.4</t>
+  </si>
+  <si>
+    <t>4.75 (0.6 %)</t>
+  </si>
+  <si>
+    <t>9.1M</t>
+  </si>
+  <si>
+    <t>Housing Development ..</t>
+  </si>
+  <si>
+    <t>2825.7</t>
+  </si>
+  <si>
+    <t>13.30 (0.5 %)</t>
+  </si>
+  <si>
+    <t>4.4M</t>
+  </si>
+  <si>
+    <t>TVS Motor Company Ltd.</t>
+  </si>
+  <si>
+    <t>547.1</t>
+  </si>
+  <si>
+    <t>2.40 (0.4 %)</t>
+  </si>
+  <si>
+    <t>Tube Investments of ..</t>
+  </si>
+  <si>
+    <t>1463.1</t>
+  </si>
+  <si>
+    <t>5.40 (0.4 %)</t>
+  </si>
+  <si>
+    <t>379.2K</t>
+  </si>
+  <si>
+    <t>193.5K</t>
+  </si>
+  <si>
+    <t>General Insurance Co..</t>
+  </si>
+  <si>
+    <t>147.8</t>
+  </si>
+  <si>
+    <t>0.55 (0.4 %)</t>
+  </si>
+  <si>
+    <t>1.5M</t>
+  </si>
+  <si>
+    <t>Bajaj Auto Ltd.</t>
+  </si>
+  <si>
+    <t>3822.2</t>
+  </si>
+  <si>
+    <t>8.70 (0.2 %)</t>
+  </si>
+  <si>
+    <t>691.5K</t>
+  </si>
+  <si>
+    <t>Bajaj Finance Ltd.</t>
+  </si>
+  <si>
+    <t>7428.8</t>
+  </si>
+  <si>
+    <t>17.30 (0.2 %)</t>
+  </si>
+  <si>
+    <t>Laurus Labs Ltd.</t>
+  </si>
+  <si>
+    <t>651.2</t>
+  </si>
+  <si>
+    <t>1.35 (0.2 %)</t>
+  </si>
+  <si>
+    <t>7.5M</t>
+  </si>
+  <si>
+    <t>3.2M</t>
+  </si>
+  <si>
+    <t>LIC Housing Finance ..</t>
+  </si>
+  <si>
+    <t>417.8</t>
+  </si>
+  <si>
+    <t>0.80 (0.2 %)</t>
+  </si>
+  <si>
+    <t>Biocon Ltd.</t>
+  </si>
+  <si>
+    <t>377.4</t>
+  </si>
+  <si>
+    <t>0.65 (0.2 %)</t>
+  </si>
+  <si>
+    <t>18.5M</t>
+  </si>
+  <si>
+    <t>5.5M</t>
+  </si>
+  <si>
+    <t>Jubilant Foodworks L..</t>
+  </si>
+  <si>
+    <t>4102.8</t>
+  </si>
+  <si>
+    <t>6.45 (0.2 %)</t>
+  </si>
+  <si>
+    <t>521.4K</t>
+  </si>
+  <si>
+    <t>Hindustan Petroleum ..</t>
+  </si>
+  <si>
+    <t>283.0</t>
+  </si>
+  <si>
+    <t>0.45 (0.2 %)</t>
+  </si>
+  <si>
+    <t>11.2M</t>
   </si>
 </sst>
 </file>
@@ -3848,7 +4808,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3871,6 +4831,1213 @@
         <v>839</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>985</v>
+      </c>
+      <c r="B2" t="s">
+        <v>986</v>
+      </c>
+      <c r="C2" t="s">
+        <v>987</v>
+      </c>
+      <c r="D2" t="s">
+        <v>988</v>
+      </c>
+      <c r="E2" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>989</v>
+      </c>
+      <c r="B3" t="s">
+        <v>990</v>
+      </c>
+      <c r="C3" t="s">
+        <v>991</v>
+      </c>
+      <c r="D3" t="s">
+        <v>992</v>
+      </c>
+      <c r="E3" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>994</v>
+      </c>
+      <c r="B4" t="s">
+        <v>995</v>
+      </c>
+      <c r="C4" t="s">
+        <v>996</v>
+      </c>
+      <c r="D4" t="s">
+        <v>997</v>
+      </c>
+      <c r="E4" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>999</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1001</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1002</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1011</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E9" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1025</v>
+      </c>
+      <c r="D10" t="s">
+        <v>932</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1029</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1040</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1045</v>
+      </c>
+      <c r="E14" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1049</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>942</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1068</v>
+      </c>
+      <c r="E19" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B20" t="s">
+        <v>881</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1076</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1081</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1086</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1090</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1095</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1096</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1100</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1101</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1111</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1115</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1116</v>
+      </c>
+      <c r="E29" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D30" t="s">
+        <v>859</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1124</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E32" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D35" t="s">
+        <v>932</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D37" t="s">
+        <v>923</v>
+      </c>
+      <c r="E37" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E38" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E39" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1163</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1168</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1169</v>
+      </c>
+      <c r="E41" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1173</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1178</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E43" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1183</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1184</v>
+      </c>
+      <c r="E44" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D45" t="s">
+        <v>919</v>
+      </c>
+      <c r="E45" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1192</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1092</v>
+      </c>
+      <c r="E46" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1197</v>
+      </c>
+      <c r="E47" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1202</v>
+      </c>
+      <c r="E48" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1206</v>
+      </c>
+      <c r="D49" t="s">
+        <v>868</v>
+      </c>
+      <c r="E49" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1209</v>
+      </c>
+      <c r="D50" t="s">
+        <v>873</v>
+      </c>
+      <c r="E50" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1212</v>
+      </c>
+      <c r="D51" t="s">
+        <v>1213</v>
+      </c>
+      <c r="E51" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1216</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1217</v>
+      </c>
+      <c r="E52" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1221</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1222</v>
+      </c>
+      <c r="E53" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D54" t="s">
+        <v>1227</v>
+      </c>
+      <c r="E54" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1232</v>
+      </c>
+      <c r="E55" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1236</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E56" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1241</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E57" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>895</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1246</v>
+      </c>
+      <c r="E58" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1250</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1251</v>
+      </c>
+      <c r="E59" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D60" t="s">
+        <v>979</v>
+      </c>
+      <c r="E60" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D61" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E61" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1264</v>
+      </c>
+      <c r="E62" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1267</v>
+      </c>
+      <c r="D63" t="s">
+        <v>859</v>
+      </c>
+      <c r="E63" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1271</v>
+      </c>
+      <c r="E64" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D65" t="s">
+        <v>959</v>
+      </c>
+      <c r="E65" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1279</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1193</v>
+      </c>
+      <c r="E66" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1283</v>
+      </c>
+      <c r="D67" t="s">
+        <v>979</v>
+      </c>
+      <c r="E67" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1286</v>
+      </c>
+      <c r="D68" t="s">
+        <v>1287</v>
+      </c>
+      <c r="E68" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D69" t="s">
+        <v>853</v>
+      </c>
+      <c r="E69" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1294</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1295</v>
+      </c>
+      <c r="E70" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1256</v>
+      </c>
+      <c r="E71" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1302</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D72" t="s">
+        <v>1304</v>
+      </c>
+      <c r="E72" t="s">
+        <v>1296</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>